<commit_message>
Solved Question not showing in some sections
</commit_message>
<xml_diff>
--- a/question/question.xlsx
+++ b/question/question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\Maths-Tutor-QT-V2\question\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB04B8D4-847B-4441-946E-DF5B7D6BD58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D92CDC0-F10D-4F93-A6C6-C7E6575A6162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -234,7 +234,7 @@
     <t>Division</t>
   </si>
   <si>
-    <t>Reminder</t>
+    <t>Remainder</t>
   </si>
 </sst>
 </file>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,7 +802,7 @@
         <v>26</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
@@ -942,7 +942,7 @@
         <v>42</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Basic Game Mode completed
</commit_message>
<xml_diff>
--- a/question/question.xlsx
+++ b/question/question.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\Maths-Tutor-QT-V2\question\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D92CDC0-F10D-4F93-A6C6-C7E6575A6162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66EF93A-D19D-47F8-BE7D-93BE735A27BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -600,7 +600,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1133,6 +1133,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FIxed error comment displayed during wrong ans
</commit_message>
<xml_diff>
--- a/question/question.xlsx
+++ b/question/question.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\Maths-Tutor-QT-V2\question\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Maths-Tutor-QT-V2\question\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66EF93A-D19D-47F8-BE7D-93BE735A27BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF9308E-4B87-4834-BC4F-495333C0BCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
   <si>
     <t>question</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>a1:10*b1:10*</t>
-  </si>
-  <si>
-    <t>{a}*+b}</t>
   </si>
   <si>
     <t>{a} % of {b} =</t>
@@ -301,9 +298,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -341,7 +338,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -447,7 +444,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -589,7 +586,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -599,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,7 +633,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -656,7 +653,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -676,7 +673,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -696,7 +693,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -716,7 +713,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -736,7 +733,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -756,7 +753,7 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -776,7 +773,7 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -796,7 +793,7 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
@@ -816,7 +813,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
@@ -836,7 +833,7 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
@@ -856,7 +853,7 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
         <v>32</v>
@@ -876,7 +873,7 @@
         <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
         <v>35</v>
@@ -896,7 +893,7 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
         <v>37</v>
@@ -905,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="F15">
         <v>5</v>
@@ -913,19 +910,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" t="s">
-        <v>40</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16">
         <v>5</v>
@@ -933,19 +930,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17">
         <v>10</v>
@@ -956,10 +953,10 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -976,10 +973,10 @@
         <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -993,19 +990,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" t="s">
         <v>45</v>
       </c>
-      <c r="B20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
         <v>46</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>47</v>
       </c>
       <c r="F20">
         <v>5</v>
@@ -1013,19 +1010,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
         <v>48</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>49</v>
       </c>
       <c r="F21">
         <v>5</v>
@@ -1033,19 +1030,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F22">
         <v>7</v>
@@ -1053,19 +1050,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F23">
         <v>7</v>
@@ -1073,19 +1070,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
         <v>52</v>
       </c>
-      <c r="B24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
         <v>53</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>54</v>
       </c>
       <c r="F24">
         <v>7</v>
@@ -1093,19 +1090,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" t="s">
         <v>55</v>
-      </c>
-      <c r="B25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" t="s">
-        <v>56</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F25">
         <v>10</v>
@@ -1113,10 +1110,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
@@ -1125,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F26">
         <v>10</v>

</xml_diff>

<commit_message>
Treading to be solved
</commit_message>
<xml_diff>
--- a/question/question.xlsx
+++ b/question/question.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Maths-Tutor-QT-V2\question\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\Maths-Tutor-QT-V2\question\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF9308E-4B87-4834-BC4F-495333C0BCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360D72E5-C25E-48AC-9517-042DA4287FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
   <si>
     <t>question</t>
   </si>
@@ -232,6 +232,18 @@
   </si>
   <si>
     <t>Remainder</t>
+  </si>
+  <si>
+    <t>Ramu has {x} apples</t>
+  </si>
+  <si>
+    <t>Bellring</t>
+  </si>
+  <si>
+    <t>x1:5</t>
+  </si>
+  <si>
+    <t>{x}</t>
   </si>
 </sst>
 </file>
@@ -298,9 +310,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -338,7 +350,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -444,7 +456,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -586,7 +598,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -594,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1128,6 +1140,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>